<commit_message>
races are now being read from txt and handled as book removed previous system and all its classes
</commit_message>
<xml_diff>
--- a/src/GameDesign/GameDesign.xlsx
+++ b/src/GameDesign/GameDesign.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Races" sheetId="1" r:id="rId1"/>
@@ -22,41 +22,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="183">
-  <si>
-    <t>Beast</t>
-  </si>
-  <si>
-    <t>Dragon</t>
-  </si>
-  <si>
-    <t>Dwarf</t>
-  </si>
-  <si>
-    <t>Elf</t>
-  </si>
-  <si>
-    <t>Ent</t>
-  </si>
-  <si>
-    <t>Giant</t>
-  </si>
-  <si>
-    <t>Gnome</t>
-  </si>
-  <si>
-    <t>Human</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="180">
   <si>
     <t>Naga</t>
   </si>
   <si>
-    <t>Necrotic</t>
-  </si>
-  <si>
-    <t>Orc</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -571,6 +541,27 @@
   </si>
   <si>
     <t>craft</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>an</t>
+  </si>
+  <si>
+    <t>Article</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>ent</t>
+  </si>
+  <si>
+    <t>naga</t>
+  </si>
+  <si>
+    <t>necrotic</t>
   </si>
 </sst>
 </file>
@@ -919,102 +910,514 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="B1:H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1"/>
+    <col min="11" max="11" width="63.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>139</v>
+      </c>
+      <c r="K1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C2">
+        <v>16</v>
+      </c>
+      <c r="D2">
+        <v>16</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>14</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>16</v>
+      </c>
+      <c r="I2">
+        <v>4</v>
+      </c>
+      <c r="J2">
+        <f>SUM(C2:I2)</f>
+        <v>70</v>
+      </c>
+      <c r="K2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>15</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <v>12</v>
+      </c>
+      <c r="I3">
+        <v>4</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J22" si="0">SUM(C3:I3)</f>
+        <v>70</v>
+      </c>
+      <c r="K3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C4">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>8</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
+      <c r="H4">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
+      <c r="I4">
+        <v>10</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="K4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C5">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>8</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>11</v>
+      </c>
+      <c r="H5">
+        <v>12</v>
+      </c>
+      <c r="I5">
+        <v>10</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="K5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C6">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>8</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>11</v>
+      </c>
+      <c r="H6">
+        <v>12</v>
+      </c>
+      <c r="I6">
+        <v>10</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="K6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" t="s">
+        <v>173</v>
+      </c>
+      <c r="C7">
+        <v>30</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>30</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="K7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>17</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H8">
+        <v>6</v>
+      </c>
+      <c r="I8">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="K8" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C9">
+        <v>14</v>
+      </c>
+      <c r="D9">
+        <v>14</v>
+      </c>
+      <c r="E9">
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="H9">
+        <v>10</v>
+      </c>
+      <c r="I9">
+        <v>8</v>
+      </c>
+      <c r="J9">
+        <f>SUM(C9:I9)</f>
+        <v>70</v>
+      </c>
+      <c r="K9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>178</v>
+      </c>
+      <c r="B10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>8</v>
+      </c>
+      <c r="F10">
+        <v>7</v>
+      </c>
+      <c r="G10">
+        <v>11</v>
+      </c>
+      <c r="H10">
+        <v>5</v>
+      </c>
+      <c r="I10">
+        <v>7</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="K10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>179</v>
+      </c>
+      <c r="B11" t="s">
+        <v>173</v>
+      </c>
+      <c r="C11">
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <v>7</v>
+      </c>
+      <c r="E11">
         <v>16</v>
       </c>
-      <c r="G1" t="s">
+      <c r="F11">
+        <v>5</v>
+      </c>
+      <c r="G11">
         <v>17</v>
       </c>
-      <c r="H1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="H11">
+        <v>8</v>
+      </c>
+      <c r="I11">
+        <v>6</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="K11" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" t="s">
+        <v>174</v>
+      </c>
+      <c r="C12">
+        <v>19</v>
+      </c>
+      <c r="D12">
+        <v>7</v>
+      </c>
+      <c r="E12">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="F12">
+        <v>8</v>
+      </c>
+      <c r="G12">
+        <v>10</v>
+      </c>
+      <c r="H12">
+        <v>19</v>
+      </c>
+      <c r="I12">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>10</v>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="K12" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J22">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1022,6 +1425,7 @@
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1053,49 +1457,49 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="E1" s="4" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="J1" s="4"/>
       <c r="K1" s="4" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3">
         <v>0.2</v>
@@ -1105,21 +1509,21 @@
         <v>0.2</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="L2" s="3">
         <v>0.1</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B3" s="3">
         <v>0.1</v>
@@ -1132,21 +1536,21 @@
         <v>0.2</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="L3" s="3">
         <v>0.1</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B4" s="3">
         <v>0.1</v>
@@ -1159,21 +1563,21 @@
         <v>0.2</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="L4" s="3">
         <v>0.1</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C5" s="3">
         <v>0.2</v>
@@ -1183,21 +1587,21 @@
         <v>0.2</v>
       </c>
       <c r="K5" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="L5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="N5" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="L5" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C6" s="3">
         <v>0.1</v>
@@ -1210,21 +1614,21 @@
         <v>0.2</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="L6" s="3">
         <v>0.1</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E7" s="3">
         <v>0.2</v>
@@ -1234,21 +1638,21 @@
         <v>0.2</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="L7" s="3">
         <v>0.1</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="D8" s="3">
         <v>0.2</v>
@@ -1258,21 +1662,21 @@
         <v>0.2</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="L8" s="3">
         <v>0.1</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="G9" s="3">
         <v>0.2</v>
@@ -1282,21 +1686,21 @@
         <v>0.2</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="L9" s="3">
         <v>0.1</v>
       </c>
       <c r="M9" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="N9" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C10" s="3">
         <v>0.1</v>
@@ -1309,21 +1713,21 @@
         <v>0.2</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="L10" s="3">
         <v>0.2</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F11" s="3">
         <v>0.2</v>
@@ -1333,21 +1737,21 @@
         <v>0.2</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="L11" s="3">
         <v>0.1</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="H12" s="3">
         <v>0.2</v>
@@ -1357,16 +1761,16 @@
         <v>0.2</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="L12" s="3">
         <v>0.1</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -1375,16 +1779,16 @@
         <v>0</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="L13" s="3">
         <v>0.1</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -1393,16 +1797,16 @@
         <v>0</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="L14" s="3">
         <v>0.1</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -1451,7 +1855,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:P30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1478,55 +1882,55 @@
   <sheetData>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="N6">
         <f t="shared" ref="N6:N21" si="0">SUM(B6:L6)</f>
@@ -1535,7 +1939,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E7">
         <v>0.2</v>
@@ -1550,7 +1954,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B8">
         <v>0.1</v>
@@ -1565,22 +1969,22 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="N9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O9" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="P9" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D10">
         <v>0.1</v>
@@ -1595,7 +1999,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="G11">
         <v>-0.2</v>
@@ -1610,7 +2014,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="K12">
         <v>-0.2</v>
@@ -1625,22 +2029,22 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="N13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O13" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="P13" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B14">
         <v>0.2</v>
@@ -1655,7 +2059,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C15">
         <v>-0.2</v>
@@ -1670,7 +2074,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D16">
         <v>0.2</v>
@@ -1685,7 +2089,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="F17">
         <v>0.2</v>
@@ -1700,7 +2104,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B18">
         <v>-0.1</v>
@@ -1715,7 +2119,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="N19">
         <f t="shared" si="0"/>
@@ -1724,7 +2128,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D20">
         <v>-0.2</v>
@@ -1739,7 +2143,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C21">
         <v>0.2</v>
@@ -1754,7 +2158,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="F22">
         <v>-0.2</v>
@@ -1765,24 +2169,24 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="C24" s="1"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="O30" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="P30" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1807,385 +2211,385 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="E5" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D6" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E6" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="E7" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="E10" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D11" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="E11" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D12" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E12" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D13" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="E13" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="C17" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="D17" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="E17" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C18" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="D18" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="E18" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C19" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="D19" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D20" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="E20" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D23" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="E23" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C24" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D24" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="E24" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C25" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="D25" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="E25" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="C26" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="D26" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="E26" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C29" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="D29" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="E29" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C30" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D30" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="E30" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C31" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="D31" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="E31" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="C32" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="D32" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="E32" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C35" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="D35" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="E35" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="C36" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="D36" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="E36" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="C37" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="D37" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="E37" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C38" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="D38" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="E38" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
professions are now read from file removed previous profession system adjusted dependent classes improved folder structure
</commit_message>
<xml_diff>
--- a/src/GameDesign/GameDesign.xlsx
+++ b/src/GameDesign/GameDesign.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Races" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="172">
   <si>
     <t>Naga</t>
   </si>
@@ -51,60 +51,6 @@
     <t>Improvisation</t>
   </si>
   <si>
-    <t>StrengthMod</t>
-  </si>
-  <si>
-    <t>EnduranceMod</t>
-  </si>
-  <si>
-    <t>KnowledgeMod</t>
-  </si>
-  <si>
-    <t>PerceptionMod</t>
-  </si>
-  <si>
-    <t>MentalityMod</t>
-  </si>
-  <si>
-    <t>HardeningMod</t>
-  </si>
-  <si>
-    <t>ImprovisationMod</t>
-  </si>
-  <si>
-    <t>Bruiser</t>
-  </si>
-  <si>
-    <t>Carnivore</t>
-  </si>
-  <si>
-    <t>Craftsman</t>
-  </si>
-  <si>
-    <t>Duelist</t>
-  </si>
-  <si>
-    <t>Farmer</t>
-  </si>
-  <si>
-    <t>Fighter</t>
-  </si>
-  <si>
-    <t>Kabbalist</t>
-  </si>
-  <si>
-    <t>Knight</t>
-  </si>
-  <si>
-    <t>Omnivore</t>
-  </si>
-  <si>
-    <t>Spiritualist</t>
-  </si>
-  <si>
-    <t>Trickster</t>
-  </si>
-  <si>
     <t>Bonus</t>
   </si>
   <si>
@@ -396,9 +342,6 @@
     <t>random effect</t>
   </si>
   <si>
-    <t>Manasteal</t>
-  </si>
-  <si>
     <t>doublecraft</t>
   </si>
   <si>
@@ -414,9 +357,6 @@
     <t>evade</t>
   </si>
   <si>
-    <t>Patotorain</t>
-  </si>
-  <si>
     <t>speedrush</t>
   </si>
   <si>
@@ -562,6 +502,42 @@
   </si>
   <si>
     <t>necrotic</t>
+  </si>
+  <si>
+    <t>strength</t>
+  </si>
+  <si>
+    <t>endurance</t>
+  </si>
+  <si>
+    <t>knowledge</t>
+  </si>
+  <si>
+    <t>perception</t>
+  </si>
+  <si>
+    <t>mentality</t>
+  </si>
+  <si>
+    <t>hardening</t>
+  </si>
+  <si>
+    <t>improvisation</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>patotorain</t>
+  </si>
+  <si>
+    <t>manasteal</t>
+  </si>
+  <si>
+    <t>article||Mod -&gt;</t>
   </si>
 </sst>
 </file>
@@ -912,7 +888,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -934,7 +910,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -958,18 +934,18 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>139</v>
+        <v>119</v>
       </c>
       <c r="K1" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="C2">
         <v>16</v>
@@ -997,15 +973,15 @@
         <v>70</v>
       </c>
       <c r="K2" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="C3">
         <v>20</v>
@@ -1033,15 +1009,15 @@
         <v>70</v>
       </c>
       <c r="K3" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="C4">
         <v>14</v>
@@ -1069,15 +1045,15 @@
         <v>70</v>
       </c>
       <c r="K4" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="B5" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="C5">
         <v>14</v>
@@ -1105,15 +1081,15 @@
         <v>70</v>
       </c>
       <c r="K5" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="B6" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="C6">
         <v>14</v>
@@ -1141,15 +1117,15 @@
         <v>70</v>
       </c>
       <c r="K6" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="C7">
         <v>30</v>
@@ -1177,15 +1153,15 @@
         <v>70</v>
       </c>
       <c r="K7" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="B8" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -1213,15 +1189,15 @@
         <v>70</v>
       </c>
       <c r="K8" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="C9">
         <v>14</v>
@@ -1249,15 +1225,15 @@
         <v>70</v>
       </c>
       <c r="K9" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="B10" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="C10">
         <v>10</v>
@@ -1285,15 +1261,15 @@
         <v>58</v>
       </c>
       <c r="K10" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="B11" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="C11">
         <v>11</v>
@@ -1321,15 +1297,15 @@
         <v>70</v>
       </c>
       <c r="K11" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="B12" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="C12">
         <v>19</v>
@@ -1357,7 +1333,7 @@
         <v>70</v>
       </c>
       <c r="K12" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1431,418 +1407,641 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="3"/>
-    <col min="2" max="2" width="13.28515625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="14" style="3" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="3.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.5703125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="17" style="3" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" style="3"/>
-    <col min="13" max="13" width="41.42578125" style="3" customWidth="1"/>
-    <col min="14" max="16384" width="11.42578125" style="3"/>
+    <col min="1" max="1" width="16.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="14" style="3" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="7.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.5703125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="17" style="3" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="3"/>
+    <col min="14" max="14" width="41.42578125" style="3" customWidth="1"/>
+    <col min="15" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>9</v>
+        <v>171</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>10</v>
+        <v>160</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>11</v>
+        <v>161</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>12</v>
+        <v>162</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>14</v>
+        <v>164</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>15</v>
+        <v>165</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>120</v>
+        <v>166</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4" t="s">
+        <v>101</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>57</v>
+        <v>102</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="3">
-        <v>0.2</v>
+        <v>43</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
       </c>
       <c r="I2" s="3">
-        <f>SUM(B2:H2)</f>
-        <v>0.2</v>
-      </c>
-      <c r="K2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3">
+        <f>SUM(C2:I2)</f>
+        <v>0.2</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="L2" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="3">
-        <v>0.1</v>
       </c>
       <c r="C3" s="3">
         <v>0.1</v>
       </c>
+      <c r="D3" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
       <c r="I3" s="3">
-        <f>SUM(B3:H3)</f>
-        <v>0.2</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="L3" s="3">
+        <v>0</v>
+      </c>
+      <c r="J3" s="3">
+        <f>SUM(C3:I3)</f>
+        <v>0.2</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C4" s="3">
         <v>0.1</v>
       </c>
-      <c r="M3" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="3">
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3">
         <v>0.1</v>
       </c>
-      <c r="H4" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I4" s="3">
-        <f t="shared" ref="I4:I18" si="0">SUM(B4:H4)</f>
-        <v>0.2</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="L4" s="3">
-        <v>0.1</v>
+      <c r="J4" s="3">
+        <f t="shared" ref="J4:J18" si="0">SUM(C4:I4)</f>
+        <v>0.2</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>19</v>
+        <v>60</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="C5" s="3">
-        <v>0.2</v>
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0</v>
       </c>
       <c r="I5" s="3">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="L5" s="3">
-        <v>0.1</v>
+        <v>0</v>
+      </c>
+      <c r="J5" s="3">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>138</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>20</v>
+        <v>94</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="C6" s="3">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="3">
         <v>0.1</v>
       </c>
+      <c r="E6" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
       <c r="I6" s="3">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="L6" s="3">
+        <v>0</v>
+      </c>
+      <c r="J6" s="3">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0</v>
+      </c>
+      <c r="J7" s="3">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0</v>
+      </c>
+      <c r="J8" s="3">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3">
         <v>0.1</v>
       </c>
-      <c r="M6" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="N6" s="3" t="s">
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0</v>
+      </c>
+      <c r="J10" s="3">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0</v>
+      </c>
+      <c r="J11" s="3">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="M11" s="3" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="I7" s="3">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="L7" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="N7" s="3" t="s">
+      <c r="N11" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="J12" s="3">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="M12" s="3" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="I8" s="3">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="L8" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="N8" s="3" t="s">
+      <c r="N12" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J13" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="M13" s="3" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="I9" s="3">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="L9" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="E10" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I10" s="3">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="L10" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="I11" s="3">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="L11" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="N11" s="3" t="s">
+      <c r="N13" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J14" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="M14" s="3" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="I12" s="3">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="L12" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="N12" s="3" t="s">
+      <c r="N14" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J15" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="3" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I13" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="L13" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="N13" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I14" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="L14" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="M14" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="N14" s="3" t="s">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J16" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M16" s="3" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I15" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L15" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I16" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L16" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="17" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I17" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L17" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="18" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I18" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L18" s="3">
-        <v>0.1</v>
+    <row r="17" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J17" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="18" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J18" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -1882,50 +2081,50 @@
   <sheetData>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1" t="s">
-        <v>139</v>
+        <v>119</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -1939,7 +2138,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="E7">
         <v>0.2</v>
@@ -1954,7 +2153,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>0.1</v>
@@ -1969,22 +2168,22 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="N9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O9" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="P9" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="D10">
         <v>0.1</v>
@@ -1999,7 +2198,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="G11">
         <v>-0.2</v>
@@ -2014,7 +2213,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="K12">
         <v>-0.2</v>
@@ -2029,22 +2228,22 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="N13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O13" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="P13" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>0.2</v>
@@ -2059,7 +2258,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="C15">
         <v>-0.2</v>
@@ -2074,7 +2273,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="D16">
         <v>0.2</v>
@@ -2089,7 +2288,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="F17">
         <v>0.2</v>
@@ -2104,7 +2303,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="B18">
         <v>-0.1</v>
@@ -2119,7 +2318,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="N19">
         <f t="shared" si="0"/>
@@ -2128,7 +2327,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D20">
         <v>-0.2</v>
@@ -2143,7 +2342,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="C21">
         <v>0.2</v>
@@ -2158,7 +2357,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="F22">
         <v>-0.2</v>
@@ -2169,24 +2368,24 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="C24" s="1"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="O30" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="P30" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2211,385 +2410,385 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="E6" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="E7" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" t="s">
         <v>50</v>
-      </c>
-      <c r="D11" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="E12" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="E13" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="C17" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="E17" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="C18" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="D18" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="E18" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="C19" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="D19" t="s">
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="D20" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="E20" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="C23" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="D23" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="E23" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="C24" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="D24" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="E24" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="C25" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="D25" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="E25" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="C26" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="D26" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="E26" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="C29" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="D29" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="E29" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="C30" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="D30" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="E30" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="C31" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="D31" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="E31" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="C32" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="D32" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="E32" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C35" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="D35" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="E35" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="C36" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="D36" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="E36" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="C37" t="s">
+        <v>79</v>
+      </c>
+      <c r="D37" t="s">
+        <v>57</v>
+      </c>
+      <c r="E37" t="s">
         <v>97</v>
-      </c>
-      <c r="D37" t="s">
-        <v>75</v>
-      </c>
-      <c r="E37" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="C38" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="D38" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="E38" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Swords no longer have attributes containg values, instead having a hashmap which receives its attributes und their names via .txt (food yet to be added this way) Adjusted slotmanagement for items and implementing new equip function for player copied player function into npc to allow testing until further implementation adjusted several tiles for better input on chooseAction
</commit_message>
<xml_diff>
--- a/src/GameDesign/GameDesign.xlsx
+++ b/src/GameDesign/GameDesign.xlsx
@@ -4,13 +4,15 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Races" sheetId="1" r:id="rId1"/>
     <sheet name="Professions" sheetId="2" r:id="rId2"/>
-    <sheet name="Traits" sheetId="3" r:id="rId3"/>
-    <sheet name="Tiles" sheetId="5" r:id="rId4"/>
+    <sheet name="WeaponMod" sheetId="6" r:id="rId3"/>
+    <sheet name="Weapons" sheetId="7" r:id="rId4"/>
+    <sheet name="Traits" sheetId="3" r:id="rId5"/>
+    <sheet name="Tiles" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="207">
   <si>
     <t>Naga</t>
   </si>
@@ -538,6 +540,111 @@
   </si>
   <si>
     <t>article||Mod -&gt;</t>
+  </si>
+  <si>
+    <t>mod</t>
+  </si>
+  <si>
+    <t>multiplier</t>
+  </si>
+  <si>
+    <t>broken</t>
+  </si>
+  <si>
+    <t>rusty</t>
+  </si>
+  <si>
+    <t>balanced</t>
+  </si>
+  <si>
+    <t>polished</t>
+  </si>
+  <si>
+    <t>improved</t>
+  </si>
+  <si>
+    <t>engraved</t>
+  </si>
+  <si>
+    <t>astonishing</t>
+  </si>
+  <si>
+    <t>damaged</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>slot</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>speed</t>
+  </si>
+  <si>
+    <t>stamina</t>
+  </si>
+  <si>
+    <t>hpReg</t>
+  </si>
+  <si>
+    <t>mpReg</t>
+  </si>
+  <si>
+    <t>armor</t>
+  </si>
+  <si>
+    <t>resistance</t>
+  </si>
+  <si>
+    <t>maxHp</t>
+  </si>
+  <si>
+    <t>maxMp</t>
+  </si>
+  <si>
+    <t>broadsword</t>
+  </si>
+  <si>
+    <t>weapon</t>
+  </si>
+  <si>
+    <t>charisma</t>
+  </si>
+  <si>
+    <t>a simple broadsword</t>
+  </si>
+  <si>
+    <t>dmg</t>
+  </si>
+  <si>
+    <t>spellDmg</t>
+  </si>
+  <si>
+    <t>effectCh.</t>
+  </si>
+  <si>
+    <t>longsword</t>
+  </si>
+  <si>
+    <t>rapier</t>
+  </si>
+  <si>
+    <t>greatsword</t>
+  </si>
+  <si>
+    <t>shortsword</t>
+  </si>
+  <si>
+    <t>scimitar</t>
+  </si>
+  <si>
+    <t>Flamberge</t>
   </si>
 </sst>
 </file>
@@ -573,12 +680,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -593,7 +706,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -606,12 +719,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF6699"/>
+      <color rgb="FFCCCCFF"/>
+      <color rgb="FFCC99FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1409,7 +1533,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -2051,6 +2175,269 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B2" s="7">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B3" s="7">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>175</v>
+      </c>
+      <c r="B4" s="7">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B5" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B6" s="7">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>178</v>
+      </c>
+      <c r="B7" s="7">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B8" s="7">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>180</v>
+      </c>
+      <c r="B9" s="7">
+        <v>1.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" customWidth="1"/>
+    <col min="6" max="6" width="4.85546875" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" customWidth="1"/>
+    <col min="8" max="8" width="9" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" customWidth="1"/>
+    <col min="11" max="11" width="6.42578125" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" customWidth="1"/>
+    <col min="13" max="13" width="6.140625" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" customWidth="1"/>
+    <col min="15" max="15" width="6.85546875" customWidth="1"/>
+    <col min="16" max="16" width="7.140625" customWidth="1"/>
+    <col min="17" max="17" width="51.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C2" s="9">
+        <v>27</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>8</v>
+      </c>
+      <c r="F2">
+        <v>20</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>5</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>206</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:P30"/>
   <sheetViews>
@@ -2394,7 +2781,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E38"/>
   <sheetViews>

</xml_diff>